<commit_message>
Add file phan chia
</commit_message>
<xml_diff>
--- a/file_Phân chia task.xlsx
+++ b/file_Phân chia task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\CyberFullStack\Front_end\Learn\7_API\Buoi25\PhoneStore_Group8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B778CA9C-FD66-4130-AE9D-9CEF4831C713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7166BBEE-7511-4535-BF37-BE3F7822029C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Page store chưa hoàn thành JS, có nhắn tin nhưng không nhận được phản hồi</t>
+  </si>
+  <si>
+    <t>Page Home</t>
   </si>
 </sst>
 </file>
@@ -132,7 +135,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +184,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -226,9 +235,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -276,6 +282,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -494,34 +501,34 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="20"/>
-    <col min="3" max="3" width="16.7109375" style="20" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="10"/>
-    <col min="5" max="5" width="16.7109375" style="21"/>
-    <col min="6" max="7" width="16.7109375" style="20"/>
-    <col min="8" max="8" width="16.7109375" style="10"/>
-    <col min="9" max="9" width="16.7109375" style="21"/>
-    <col min="10" max="10" width="85.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="16.7109375" style="10"/>
+    <col min="1" max="1" width="27.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="19"/>
+    <col min="3" max="3" width="16.7109375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="9"/>
+    <col min="5" max="5" width="16.7109375" style="20"/>
+    <col min="6" max="7" width="16.7109375" style="19"/>
+    <col min="8" max="8" width="16.7109375" style="9"/>
+    <col min="9" max="9" width="16.7109375" style="20"/>
+    <col min="10" max="10" width="85.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="16.7109375" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -547,348 +554,435 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="12">
-        <v>45007</v>
-      </c>
-      <c r="C2" s="12">
-        <v>45007</v>
-      </c>
-      <c r="D2" s="13">
-        <v>1</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="15"/>
+      <c r="B2" s="11">
+        <v>45007</v>
+      </c>
+      <c r="C2" s="11">
+        <v>45007</v>
+      </c>
+      <c r="D2" s="12">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="15">
+        <v>45007</v>
+      </c>
+      <c r="C3" s="15">
+        <v>45007</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="11">
+        <v>45007</v>
+      </c>
+      <c r="G3" s="11">
+        <v>45007</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15"/>
-    </row>
-    <row r="4" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B5" s="15">
         <v>45002</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C5" s="15">
         <v>45002</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D5" s="12">
         <v>0.9</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="12">
-        <v>45007</v>
-      </c>
-      <c r="G4" s="12">
-        <v>45007</v>
-      </c>
-      <c r="H4" s="13">
-        <v>1</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="15"/>
-    </row>
-    <row r="5" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="E5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="11">
+        <v>45007</v>
+      </c>
+      <c r="G5" s="11">
+        <v>45007</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B6" s="11">
         <v>45003</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C6" s="11">
         <v>45003</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D6" s="12">
         <v>0.9</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="12">
-        <v>45007</v>
-      </c>
-      <c r="G5" s="12">
-        <v>45007</v>
-      </c>
-      <c r="H5" s="13">
-        <v>1</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="E6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="11">
+        <v>45007</v>
+      </c>
+      <c r="G6" s="11">
+        <v>45007</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B7" s="11">
         <v>45004</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C7" s="11">
         <v>45004</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D7" s="12">
         <v>0.9</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="12">
-        <v>45007</v>
-      </c>
-      <c r="G6" s="12">
-        <v>45007</v>
-      </c>
-      <c r="H6" s="13">
-        <v>1</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="E7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="11">
+        <v>45007</v>
+      </c>
+      <c r="G7" s="11">
+        <v>45007</v>
+      </c>
+      <c r="H7" s="12">
+        <v>1</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B8" s="15">
         <v>45005</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C8" s="15">
         <v>45005</v>
       </c>
-      <c r="D7" s="13">
-        <v>1</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="D8" s="12">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="11">
         <v>45006</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G8" s="11">
         <v>45006</v>
       </c>
-      <c r="H7" s="13">
-        <v>1</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="15"/>
-    </row>
-    <row r="8" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
+      <c r="H8" s="12">
+        <v>1</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B9" s="11">
         <v>45008</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C9" s="11">
         <v>45008</v>
       </c>
-      <c r="D8" s="13">
-        <v>1</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="12">
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="11">
         <v>45008</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G9" s="11">
         <v>45008</v>
       </c>
-      <c r="H8" s="13">
-        <v>1</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="15"/>
-    </row>
-    <row r="9" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="H9" s="12">
+        <v>1</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B10" s="11">
         <v>45009</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C10" s="11">
         <v>45009</v>
       </c>
-      <c r="D9" s="13">
-        <v>1</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="12">
+      <c r="D10" s="12">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="11">
         <v>45009</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G10" s="11">
         <v>45009</v>
       </c>
-      <c r="H9" s="13">
-        <v>1</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
+      <c r="H10" s="12">
+        <v>1</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B11" s="11">
         <v>45009</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C11" s="11">
         <v>45011</v>
       </c>
-      <c r="D10" s="13">
-        <v>1</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="12">
+      <c r="D11" s="12">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="11">
         <v>45011</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G11" s="11">
         <v>45011</v>
       </c>
-      <c r="H10" s="13">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="H11" s="12">
+        <v>1</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="6"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="15"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="15"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="11"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B15" s="15">
         <v>45018</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C15" s="15">
         <v>45018</v>
       </c>
-      <c r="D16" s="18">
-        <v>1</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="16">
+      <c r="D15" s="17">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="15">
         <v>45018</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G15" s="15">
         <v>45018</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H15" s="17">
         <v>0.6</v>
       </c>
-      <c r="I16" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="11" t="s">
+      <c r="I15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="10" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="17" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="I25" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>